<commit_message>
added SVM to detect patterns in cc
</commit_message>
<xml_diff>
--- a/assets/sample_data_1.xlsx
+++ b/assets/sample_data_1.xlsx
@@ -9,11 +9,12 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="17256" windowHeight="7812"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="17256" windowHeight="7812" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="X bar and R chart" sheetId="1" r:id="rId1"/>
     <sheet name="C chart" sheetId="2" r:id="rId2"/>
+    <sheet name="U chart" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -25,9 +26,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="1">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="2">
   <si>
     <t>Sample</t>
+  </si>
+  <si>
+    <t>sample_size</t>
   </si>
 </sst>
 </file>
@@ -348,7 +352,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="I16" sqref="I16"/>
     </sheetView>
   </sheetViews>
@@ -685,7 +689,7 @@
   <dimension ref="A1:B11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G7" sqref="E2:G7"/>
+      <selection activeCell="E27" sqref="E27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -781,4 +785,250 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C21"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2">
+        <v>52</v>
+      </c>
+      <c r="C2">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3">
+        <v>48</v>
+      </c>
+      <c r="C3">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4">
+        <v>56</v>
+      </c>
+      <c r="C4">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5">
+        <v>25</v>
+      </c>
+      <c r="C5">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6">
+        <v>39</v>
+      </c>
+      <c r="C6">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7">
+        <v>39</v>
+      </c>
+      <c r="C7">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8">
+        <v>54</v>
+      </c>
+      <c r="C8">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9">
+        <v>70</v>
+      </c>
+      <c r="C9">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10">
+        <v>41</v>
+      </c>
+      <c r="C10">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A11">
+        <v>10</v>
+      </c>
+      <c r="B11">
+        <v>43</v>
+      </c>
+      <c r="C11">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A12">
+        <v>11</v>
+      </c>
+      <c r="B12">
+        <v>47</v>
+      </c>
+      <c r="C12">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A13">
+        <v>12</v>
+      </c>
+      <c r="B13">
+        <v>52</v>
+      </c>
+      <c r="C13">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A14">
+        <v>13</v>
+      </c>
+      <c r="B14">
+        <v>44</v>
+      </c>
+      <c r="C14">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A15">
+        <v>14</v>
+      </c>
+      <c r="B15">
+        <v>47</v>
+      </c>
+      <c r="C15">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A16">
+        <v>15</v>
+      </c>
+      <c r="B16">
+        <v>50</v>
+      </c>
+      <c r="C16">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A17">
+        <v>16</v>
+      </c>
+      <c r="B17">
+        <v>40</v>
+      </c>
+      <c r="C17">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A18">
+        <v>17</v>
+      </c>
+      <c r="B18">
+        <v>47</v>
+      </c>
+      <c r="C18">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A19">
+        <v>18</v>
+      </c>
+      <c r="B19">
+        <v>46</v>
+      </c>
+      <c r="C19">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A20">
+        <v>19</v>
+      </c>
+      <c r="B20">
+        <v>44</v>
+      </c>
+      <c r="C20">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A21">
+        <v>20</v>
+      </c>
+      <c r="B21">
+        <v>50</v>
+      </c>
+      <c r="C21">
+        <v>110</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>